<commit_message>
Mise à jour de la matrice
</commit_message>
<xml_diff>
--- a/Merise/Matrice des dépendances fonctionnelles.xlsx
+++ b/Merise/Matrice des dépendances fonctionnelles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>Quantité vendue</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Nom del' objet vendu</t>
   </si>
   <si>
-    <t>Prix de l'objet</t>
-  </si>
-  <si>
     <t>Nom de l'objet vendu</t>
   </si>
   <si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>Ville de vente</t>
+  </si>
+  <si>
+    <t>Prix de l'objet en obelos d'or</t>
+  </si>
+  <si>
+    <t>Prix de l'objet en obelos d'argent</t>
+  </si>
+  <si>
+    <t>Prix de l'objet en obelos de fer</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,197 +415,227 @@
     <col min="13" max="13" width="3.5546875" customWidth="1"/>
     <col min="14" max="14" width="3.21875" customWidth="1"/>
     <col min="15" max="15" width="2.88671875" customWidth="1"/>
+    <col min="16" max="16" width="3.21875" customWidth="1"/>
+    <col min="17" max="17" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>